<commit_message>
fixed typo in source file; 'NCRN_MONO_VCCR' had an extra space: 'NCRN_MONO_ VCCR', which was causing joins to fail
</commit_message>
<xml_diff>
--- a/data/bob/nps_spring_habitat_2022_bob.xlsx
+++ b/data/bob/nps_spring_habitat_2022_bob.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Data\Small stuff\Bob\BOB\DOCS\proposals\NPS NCR monitoring 2019\sampling 2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwainright\OneDrive - DOI\Documents\data_projects\2023\iss156_bss_edd\data\bob\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F388BC-1A81-4476-9FDD-1797EDE86125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24270" windowHeight="11670" tabRatio="500"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Spring" sheetId="1" r:id="rId1"/>
@@ -167,9 +168,6 @@
     <t>NCRN_MANA_YOBR</t>
   </si>
   <si>
-    <t>NCRN_MONO_ VCCR</t>
-  </si>
-  <si>
     <t>NCRN_MONO_BUCK</t>
   </si>
   <si>
@@ -447,14 +445,17 @@
   </si>
   <si>
     <t>Turkey Run</t>
+  </si>
+  <si>
+    <t>NCRN_MONO_VCCR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -529,19 +530,19 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -821,144 +822,144 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BO51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1890" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1890" topLeftCell="A10" activePane="bottomLeft"/>
       <selection activeCell="M2" sqref="M1:M1048576"/>
-      <selection pane="bottomLeft" activeCell="M19" sqref="M19"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="1" max="1" width="31.5" style="3" customWidth="1"/>
-    <col min="2" max="13" width="14.125" style="7" customWidth="1"/>
-    <col min="20" max="20" width="11.375" style="3" customWidth="1"/>
-    <col min="24" max="24" width="10.875" style="3"/>
-    <col min="26" max="26" width="10.875" style="3"/>
-    <col min="32" max="32" width="10.875" style="3"/>
-    <col min="38" max="38" width="10.875" style="3"/>
-    <col min="43" max="43" width="10.875" style="3"/>
+    <col min="2" max="13" width="14.09765625" style="7" customWidth="1"/>
+    <col min="20" max="20" width="11.34765625" style="3" customWidth="1"/>
+    <col min="24" max="24" width="10.84765625" style="3"/>
+    <col min="26" max="26" width="10.84765625" style="3"/>
+    <col min="32" max="32" width="10.84765625" style="3"/>
+    <col min="38" max="38" width="10.84765625" style="3"/>
+    <col min="43" max="43" width="10.84765625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:67" x14ac:dyDescent="0.6">
       <c r="F1" s="3"/>
-      <c r="G1" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="15" t="s">
+      <c r="G1" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="15" t="s">
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13"/>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="15" t="s">
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="Z1" s="14"/>
-      <c r="AA1" s="15" t="s">
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="AB1" s="16"/>
-      <c r="AC1" s="16"/>
-      <c r="AD1" s="16"/>
-      <c r="AE1" s="16"/>
-      <c r="AF1" s="16"/>
-      <c r="AG1" s="16"/>
-      <c r="AH1" s="16"/>
-      <c r="AI1" s="16"/>
-      <c r="AJ1" s="16"/>
-      <c r="AK1" s="16"/>
-      <c r="AL1" s="16"/>
-      <c r="AM1" s="13" t="s">
+      <c r="AB1" s="17"/>
+      <c r="AC1" s="17"/>
+      <c r="AD1" s="17"/>
+      <c r="AE1" s="17"/>
+      <c r="AF1" s="17"/>
+      <c r="AG1" s="17"/>
+      <c r="AH1" s="17"/>
+      <c r="AI1" s="17"/>
+      <c r="AJ1" s="17"/>
+      <c r="AK1" s="17"/>
+      <c r="AL1" s="17"/>
+      <c r="AM1" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="AN1" s="13"/>
-      <c r="AO1" s="13"/>
-      <c r="AP1" s="13"/>
-      <c r="AQ1" s="14"/>
-      <c r="AR1" s="15" t="s">
+      <c r="AN1" s="15"/>
+      <c r="AO1" s="15"/>
+      <c r="AP1" s="15"/>
+      <c r="AQ1" s="16"/>
+      <c r="AR1" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="AS1" s="15"/>
+      <c r="AT1" s="15"/>
+      <c r="AU1" s="15"/>
+      <c r="AV1" s="15"/>
+      <c r="AW1" s="15"/>
+      <c r="AX1" s="15"/>
+      <c r="AY1" s="15"/>
+      <c r="AZ1" s="15"/>
+      <c r="BA1" s="15"/>
+      <c r="BB1" s="15"/>
+      <c r="BC1" s="15"/>
+      <c r="BD1" s="15"/>
+      <c r="BE1" s="15"/>
+      <c r="BF1" s="15"/>
+      <c r="BG1" s="15"/>
+      <c r="BH1" s="15"/>
+      <c r="BI1" s="15"/>
+      <c r="BJ1" s="15"/>
+      <c r="BK1" s="15"/>
+      <c r="BL1" s="15"/>
+      <c r="BM1" s="15"/>
+      <c r="BN1" s="15"/>
+      <c r="BO1" s="16"/>
+    </row>
+    <row r="2" spans="1:67" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="K2" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="AS1" s="13"/>
-      <c r="AT1" s="13"/>
-      <c r="AU1" s="13"/>
-      <c r="AV1" s="13"/>
-      <c r="AW1" s="13"/>
-      <c r="AX1" s="13"/>
-      <c r="AY1" s="13"/>
-      <c r="AZ1" s="13"/>
-      <c r="BA1" s="13"/>
-      <c r="BB1" s="13"/>
-      <c r="BC1" s="13"/>
-      <c r="BD1" s="13"/>
-      <c r="BE1" s="13"/>
-      <c r="BF1" s="13"/>
-      <c r="BG1" s="13"/>
-      <c r="BH1" s="13"/>
-      <c r="BI1" s="13"/>
-      <c r="BJ1" s="13"/>
-      <c r="BK1" s="13"/>
-      <c r="BL1" s="13"/>
-      <c r="BM1" s="13"/>
-      <c r="BN1" s="13"/>
-      <c r="BO1" s="14"/>
-    </row>
-    <row r="2" spans="1:67" ht="63" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="K2" s="8" t="s">
+      <c r="L2" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="8" t="s">
         <v>91</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>92</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>1</v>
@@ -1051,79 +1052,79 @@
         <v>33</v>
       </c>
       <c r="AR2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AS2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AT2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="AU2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AV2" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="AS2" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="AT2" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="AU2" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="AV2" s="4" t="s">
+      <c r="AW2" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="AW2" s="4" t="s">
+      <c r="AX2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="AX2" s="4" t="s">
+      <c r="AY2" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="AY2" s="4" t="s">
+      <c r="AZ2" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="AZ2" s="4" t="s">
+      <c r="BA2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="BA2" s="4" t="s">
+      <c r="BB2" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="BB2" s="4" t="s">
+      <c r="BC2" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="BC2" s="4" t="s">
+      <c r="BD2" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="BD2" s="4" t="s">
+      <c r="BE2" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="BE2" s="4" t="s">
+      <c r="BF2" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="BF2" s="4" t="s">
+      <c r="BG2" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="BG2" s="4" t="s">
+      <c r="BH2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="BH2" s="4" t="s">
+      <c r="BI2" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="BI2" s="4" t="s">
+      <c r="BJ2" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="BJ2" s="4" t="s">
+      <c r="BK2" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="BK2" s="4" t="s">
+      <c r="BL2" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="BL2" s="4" t="s">
+      <c r="BM2" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="BM2" s="4" t="s">
+      <c r="BN2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="BN2" s="4" t="s">
+      <c r="BO2" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="BO2" s="5" t="s">
-        <v>83</v>
-      </c>
     </row>
-    <row r="3" spans="1:67" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:67" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A3" s="3" t="s">
         <v>36</v>
       </c>
@@ -1134,31 +1135,31 @@
         <v>0.77083333333333337</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="M3" s="17">
+        <v>58</v>
+      </c>
+      <c r="M3" s="13">
         <v>5.2266666666666666</v>
       </c>
       <c r="N3" s="1">
@@ -1168,73 +1169,73 @@
         <v>12</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q3" s="1">
         <v>10</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U3" s="1">
         <v>8</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB3" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC3" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD3" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE3" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF3" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG3" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AH3" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AI3" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AJ3" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AK3" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AL3" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AM3">
         <v>20</v>
@@ -1252,10 +1253,10 @@
         <v>0</v>
       </c>
       <c r="AR3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AS3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AT3">
         <v>1</v>
@@ -1264,10 +1265,10 @@
         <v>2</v>
       </c>
       <c r="AV3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AW3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AX3">
         <v>1</v>
@@ -1276,10 +1277,10 @@
         <v>2</v>
       </c>
       <c r="AZ3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BA3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BB3">
         <v>1</v>
@@ -1288,10 +1289,10 @@
         <v>2</v>
       </c>
       <c r="BD3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BE3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BF3">
         <v>1</v>
@@ -1300,10 +1301,10 @@
         <v>2</v>
       </c>
       <c r="BH3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BI3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BJ3">
         <v>1</v>
@@ -1312,10 +1313,10 @@
         <v>2</v>
       </c>
       <c r="BL3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BM3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BN3">
         <v>1</v>
@@ -1324,7 +1325,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:67" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:67" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A4" s="3" t="s">
         <v>37</v>
       </c>
@@ -1335,33 +1336,33 @@
         <v>0.44791666666666669</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="M4" s="17">
+        <v>58</v>
+      </c>
+      <c r="M4" s="13">
         <v>8.4533333333333349</v>
       </c>
       <c r="N4" s="1">
@@ -1371,73 +1372,73 @@
         <v>20</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q4" s="1">
         <v>50</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U4" s="1">
         <v>20</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AA4" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB4" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC4" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD4" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE4" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG4" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AH4" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AI4" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AJ4" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AK4" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AL4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AM4">
         <v>20</v>
@@ -1455,10 +1456,10 @@
         <v>0</v>
       </c>
       <c r="AR4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AS4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AT4">
         <v>1</v>
@@ -1467,10 +1468,10 @@
         <v>2</v>
       </c>
       <c r="AV4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AW4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AX4">
         <v>1</v>
@@ -1479,10 +1480,10 @@
         <v>2</v>
       </c>
       <c r="AZ4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="BA4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BB4">
         <v>1</v>
@@ -1491,10 +1492,10 @@
         <v>2</v>
       </c>
       <c r="BD4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="BE4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BF4">
         <v>1</v>
@@ -1503,10 +1504,10 @@
         <v>2</v>
       </c>
       <c r="BH4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="BI4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BJ4">
         <v>1</v>
@@ -1515,10 +1516,10 @@
         <v>2</v>
       </c>
       <c r="BL4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="BM4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BN4">
         <v>1</v>
@@ -1527,7 +1528,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:67" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:67" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A5" s="3" t="s">
         <v>38</v>
       </c>
@@ -1538,33 +1539,33 @@
         <v>0.34722222222222227</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="F5" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="M5" s="17">
+        <v>58</v>
+      </c>
+      <c r="M5" s="13">
         <v>6.9733333333333327</v>
       </c>
       <c r="N5" s="1">
@@ -1574,73 +1575,73 @@
         <v>20</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q5" s="1">
         <v>20</v>
       </c>
       <c r="R5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S5" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="S5" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="T5" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U5" s="1">
         <v>50</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z5" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AA5" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB5" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC5" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD5" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE5" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF5" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG5" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AH5" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AI5" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AJ5" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AK5" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AL5" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AM5">
         <v>20</v>
@@ -1658,10 +1659,10 @@
         <v>0</v>
       </c>
       <c r="AR5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AS5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AT5">
         <v>1</v>
@@ -1670,10 +1671,10 @@
         <v>2</v>
       </c>
       <c r="AV5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AW5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AX5">
         <v>1</v>
@@ -1682,10 +1683,10 @@
         <v>2</v>
       </c>
       <c r="AZ5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BA5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BB5">
         <v>1</v>
@@ -1694,10 +1695,10 @@
         <v>2</v>
       </c>
       <c r="BD5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BE5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BF5">
         <v>1</v>
@@ -1706,10 +1707,10 @@
         <v>2</v>
       </c>
       <c r="BH5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BI5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BJ5">
         <v>1</v>
@@ -1718,10 +1719,10 @@
         <v>2</v>
       </c>
       <c r="BL5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BM5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BN5">
         <v>1</v>
@@ -1730,7 +1731,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:67" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:67" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A6" s="3" t="s">
         <v>39</v>
       </c>
@@ -1741,33 +1742,33 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="G6" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="M6" s="17">
+        <v>58</v>
+      </c>
+      <c r="M6" s="13">
         <v>4.84</v>
       </c>
       <c r="N6" s="1">
@@ -1777,73 +1778,73 @@
         <v>20</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q6" s="1">
         <v>50</v>
       </c>
       <c r="R6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S6" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="S6" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="T6" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U6" s="1">
         <v>50</v>
       </c>
       <c r="V6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W6" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="W6" s="1" t="s">
+      <c r="X6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z6" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="X6" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y6" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z6" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="AA6" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB6" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC6" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD6" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE6" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF6" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG6" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AH6" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AI6" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AJ6" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AK6" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AL6" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AM6">
         <v>20</v>
@@ -1861,10 +1862,10 @@
         <v>0</v>
       </c>
       <c r="AR6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AS6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AT6">
         <v>1</v>
@@ -1873,10 +1874,10 @@
         <v>2</v>
       </c>
       <c r="AV6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AW6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AX6">
         <v>1</v>
@@ -1885,10 +1886,10 @@
         <v>2</v>
       </c>
       <c r="AZ6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BA6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BB6">
         <v>1</v>
@@ -1897,10 +1898,10 @@
         <v>2</v>
       </c>
       <c r="BD6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BE6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BF6">
         <v>1</v>
@@ -1909,10 +1910,10 @@
         <v>2</v>
       </c>
       <c r="BH6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BI6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BJ6">
         <v>1</v>
@@ -1921,10 +1922,10 @@
         <v>2</v>
       </c>
       <c r="BL6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BM6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BN6">
         <v>1</v>
@@ -1933,7 +1934,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:67" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:67" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A7" s="3" t="s">
         <v>40</v>
       </c>
@@ -1944,31 +1945,31 @@
         <v>0.70138888888888884</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="M7" s="17">
+        <v>58</v>
+      </c>
+      <c r="M7" s="13">
         <v>18.786666666666665</v>
       </c>
       <c r="N7" s="1">
@@ -1978,73 +1979,73 @@
         <v>19</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q7" s="1">
         <v>20</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U7" s="1">
         <v>15</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="X7" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z7" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AA7" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB7" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC7" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD7" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE7" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF7" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG7" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AH7" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AI7" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AJ7" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AK7" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AL7" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AM7">
         <v>20</v>
@@ -2062,10 +2063,10 @@
         <v>0</v>
       </c>
       <c r="AR7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AS7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AT7">
         <v>1</v>
@@ -2074,10 +2075,10 @@
         <v>2</v>
       </c>
       <c r="AV7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AW7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AX7">
         <v>1</v>
@@ -2086,10 +2087,10 @@
         <v>2</v>
       </c>
       <c r="AZ7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BA7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="BB7">
         <v>1</v>
@@ -2098,10 +2099,10 @@
         <v>2</v>
       </c>
       <c r="BD7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BE7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="BF7">
         <v>1</v>
@@ -2110,10 +2111,10 @@
         <v>2</v>
       </c>
       <c r="BH7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BI7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="BJ7">
         <v>1</v>
@@ -2122,10 +2123,10 @@
         <v>2</v>
       </c>
       <c r="BL7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BM7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="BN7">
         <v>1</v>
@@ -2134,7 +2135,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:67" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:67" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A8" s="3" t="s">
         <v>41</v>
       </c>
@@ -2145,31 +2146,31 @@
         <v>0.48958333333333331</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="M8" s="17">
+        <v>58</v>
+      </c>
+      <c r="M8" s="13">
         <v>4</v>
       </c>
       <c r="N8" s="1">
@@ -2179,73 +2180,73 @@
         <v>19</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q8" s="1">
         <v>50</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U8" s="1">
         <v>50</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="X8" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z8" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AA8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB8" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC8" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD8" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE8" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF8" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG8" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AH8" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AI8" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AJ8" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AK8" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AL8" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AM8">
         <v>20</v>
@@ -2263,10 +2264,10 @@
         <v>0</v>
       </c>
       <c r="AR8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AS8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AT8">
         <v>1</v>
@@ -2275,10 +2276,10 @@
         <v>1</v>
       </c>
       <c r="AV8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AW8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AX8">
         <v>1</v>
@@ -2287,10 +2288,10 @@
         <v>1</v>
       </c>
       <c r="AZ8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BA8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="BB8">
         <v>1</v>
@@ -2299,10 +2300,10 @@
         <v>2</v>
       </c>
       <c r="BD8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BE8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="BF8">
         <v>1</v>
@@ -2311,10 +2312,10 @@
         <v>2</v>
       </c>
       <c r="BH8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BI8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="BJ8">
         <v>1</v>
@@ -2323,10 +2324,10 @@
         <v>2</v>
       </c>
       <c r="BL8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BM8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="BN8">
         <v>1</v>
@@ -2335,7 +2336,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:67" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:67" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A9" s="3" t="s">
         <v>42</v>
       </c>
@@ -2346,31 +2347,31 @@
         <v>0.44791666666666669</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="M9" s="17">
+        <v>58</v>
+      </c>
+      <c r="M9" s="13">
         <v>6.8400000000000016</v>
       </c>
       <c r="N9" s="1">
@@ -2380,73 +2381,73 @@
         <v>17</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q9" s="1">
         <v>40</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U9" s="1">
         <v>8</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="X9" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y9" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z9" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AA9" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB9" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC9" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD9" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE9" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF9" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG9" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AH9" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AI9" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AJ9" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AK9" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AL9" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AM9">
         <v>20</v>
@@ -2464,10 +2465,10 @@
         <v>0</v>
       </c>
       <c r="AR9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AS9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AT9">
         <v>1</v>
@@ -2476,10 +2477,10 @@
         <v>2</v>
       </c>
       <c r="AV9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AW9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AX9">
         <v>2</v>
@@ -2488,10 +2489,10 @@
         <v>2</v>
       </c>
       <c r="AZ9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BA9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BB9">
         <v>1</v>
@@ -2500,10 +2501,10 @@
         <v>2</v>
       </c>
       <c r="BD9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BE9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BF9">
         <v>1</v>
@@ -2512,10 +2513,10 @@
         <v>2</v>
       </c>
       <c r="BH9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BI9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BJ9">
         <v>1</v>
@@ -2524,10 +2525,10 @@
         <v>1</v>
       </c>
       <c r="BL9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BM9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="BN9">
         <v>1</v>
@@ -2536,7 +2537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:67" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:67" ht="32.25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A10" s="3" t="s">
         <v>43</v>
       </c>
@@ -2547,31 +2548,31 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="M10" s="17">
+        <v>58</v>
+      </c>
+      <c r="M10" s="13">
         <v>7.5199999999999987</v>
       </c>
       <c r="N10" s="1">
@@ -2581,73 +2582,73 @@
         <v>18</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q10" s="1">
         <v>40</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U10" s="1">
         <v>40</v>
       </c>
       <c r="V10" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="W10" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="X10" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y10" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z10" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AA10" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB10" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC10" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD10" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE10" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF10" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG10" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AH10" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AI10" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AJ10" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AK10" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AL10" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AM10">
         <v>20</v>
@@ -2665,10 +2666,10 @@
         <v>0</v>
       </c>
       <c r="AR10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AS10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AT10">
         <v>1</v>
@@ -2677,10 +2678,10 @@
         <v>2</v>
       </c>
       <c r="AV10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AW10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AX10">
         <v>1</v>
@@ -2689,10 +2690,10 @@
         <v>2</v>
       </c>
       <c r="AZ10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BA10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BB10">
         <v>1</v>
@@ -2701,10 +2702,10 @@
         <v>2</v>
       </c>
       <c r="BD10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BE10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BF10">
         <v>1</v>
@@ -2713,10 +2714,10 @@
         <v>2</v>
       </c>
       <c r="BH10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BI10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BJ10">
         <v>1</v>
@@ -2725,10 +2726,10 @@
         <v>1</v>
       </c>
       <c r="BL10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BM10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BN10">
         <v>1</v>
@@ -2737,7 +2738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:67" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:67" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A11" s="3" t="s">
         <v>44</v>
       </c>
@@ -2748,31 +2749,31 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="M11" s="17">
+        <v>58</v>
+      </c>
+      <c r="M11" s="13">
         <v>0.66666666666666674</v>
       </c>
       <c r="N11" s="1">
@@ -2782,73 +2783,73 @@
         <v>17</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q11" s="1">
         <v>30</v>
       </c>
       <c r="R11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S11" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="S11" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="T11" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U11" s="1">
         <v>50</v>
       </c>
       <c r="V11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W11" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="W11" s="1" t="s">
+      <c r="X11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z11" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="X11" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y11" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z11" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="AA11" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB11" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC11" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD11" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE11" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF11" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG11" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AH11" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AI11" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AJ11" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AK11" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AL11" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AM11">
         <v>20</v>
@@ -2866,10 +2867,10 @@
         <v>0</v>
       </c>
       <c r="AR11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AS11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AT11">
         <v>1</v>
@@ -2878,10 +2879,10 @@
         <v>2</v>
       </c>
       <c r="AV11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AW11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AX11">
         <v>1</v>
@@ -2890,10 +2891,10 @@
         <v>2</v>
       </c>
       <c r="AZ11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="BA11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BB11">
         <v>1</v>
@@ -2902,10 +2903,10 @@
         <v>1</v>
       </c>
       <c r="BD11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="BE11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BF11">
         <v>1</v>
@@ -2914,10 +2915,10 @@
         <v>1</v>
       </c>
       <c r="BH11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="BI11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BJ11">
         <v>1</v>
@@ -2926,10 +2927,10 @@
         <v>1</v>
       </c>
       <c r="BL11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="BM11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BN11">
         <v>1</v>
@@ -2938,7 +2939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:67" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:67" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A12" s="3" t="s">
         <v>45</v>
       </c>
@@ -2949,31 +2950,31 @@
         <v>0.625</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="M12" s="17">
+        <v>58</v>
+      </c>
+      <c r="M12" s="13">
         <v>0.60000000000000031</v>
       </c>
       <c r="N12" s="1">
@@ -2983,73 +2984,73 @@
         <v>17</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q12" s="1">
         <v>50</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U12" s="1">
         <v>50</v>
       </c>
       <c r="V12" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="X12" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y12" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z12" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AA12" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB12" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC12" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD12" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE12" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF12" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG12" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AH12" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AI12" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AJ12" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AK12" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AL12" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AM12">
         <v>20</v>
@@ -3067,10 +3068,10 @@
         <v>0</v>
       </c>
       <c r="AR12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AS12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AT12">
         <v>1</v>
@@ -3079,10 +3080,10 @@
         <v>2</v>
       </c>
       <c r="AV12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AW12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AX12">
         <v>1</v>
@@ -3091,10 +3092,10 @@
         <v>2</v>
       </c>
       <c r="AZ12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BA12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BB12">
         <v>2</v>
@@ -3103,10 +3104,10 @@
         <v>1</v>
       </c>
       <c r="BD12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BE12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BF12">
         <v>2</v>
@@ -3115,10 +3116,10 @@
         <v>1</v>
       </c>
       <c r="BH12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BI12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BJ12">
         <v>2</v>
@@ -3127,10 +3128,10 @@
         <v>1</v>
       </c>
       <c r="BL12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BM12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BN12">
         <v>2</v>
@@ -3139,9 +3140,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:67" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:67" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A13" s="3" t="s">
-        <v>46</v>
+        <v>139</v>
       </c>
       <c r="B13" s="9">
         <v>44637</v>
@@ -3150,31 +3151,31 @@
         <v>0.61111111111111105</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="M13" s="17">
+        <v>58</v>
+      </c>
+      <c r="M13" s="13">
         <v>2.6933333333333325</v>
       </c>
       <c r="N13" s="1">
@@ -3184,73 +3185,73 @@
         <v>20</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q13" s="1">
         <v>20</v>
       </c>
       <c r="R13" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="S13" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="S13" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="T13" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U13" s="1">
         <v>50</v>
       </c>
       <c r="V13" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="X13" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y13" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z13" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AA13" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB13" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC13" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD13" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE13" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF13" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG13" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AH13" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AI13" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AJ13" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AK13" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AL13" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AM13">
         <v>20</v>
@@ -3268,10 +3269,10 @@
         <v>0</v>
       </c>
       <c r="AR13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AS13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AT13">
         <v>1</v>
@@ -3280,10 +3281,10 @@
         <v>2</v>
       </c>
       <c r="AV13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AW13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AX13">
         <v>1</v>
@@ -3292,10 +3293,10 @@
         <v>2</v>
       </c>
       <c r="AZ13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BA13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="BB13">
         <v>1</v>
@@ -3304,10 +3305,10 @@
         <v>1</v>
       </c>
       <c r="BD13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BE13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="BF13">
         <v>1</v>
@@ -3316,10 +3317,10 @@
         <v>1</v>
       </c>
       <c r="BH13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BI13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="BJ13">
         <v>1</v>
@@ -3328,10 +3329,10 @@
         <v>2</v>
       </c>
       <c r="BL13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BM13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="BN13">
         <v>1</v>
@@ -3340,9 +3341,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:67" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:67" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A14" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14" s="9">
         <v>44637</v>
@@ -3351,31 +3352,31 @@
         <v>0.5625</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="M14" s="17">
+        <v>58</v>
+      </c>
+      <c r="M14" s="13">
         <v>1.8000000000000005</v>
       </c>
       <c r="N14">
@@ -3385,73 +3386,73 @@
         <v>20</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q14" s="1">
         <v>50</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T14" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U14" s="1">
         <v>5</v>
       </c>
       <c r="V14" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="W14" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="W14" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="X14" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Y14" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z14" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AA14" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB14" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC14" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD14" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE14" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF14" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG14" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AH14" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AI14" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AJ14" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AK14" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AL14" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AM14">
         <v>20</v>
@@ -3469,10 +3470,10 @@
         <v>0</v>
       </c>
       <c r="AR14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AS14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AT14">
         <v>2</v>
@@ -3481,10 +3482,10 @@
         <v>1</v>
       </c>
       <c r="AV14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AW14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AX14">
         <v>1</v>
@@ -3493,10 +3494,10 @@
         <v>2</v>
       </c>
       <c r="AZ14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BA14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BB14">
         <v>1</v>
@@ -3505,10 +3506,10 @@
         <v>1</v>
       </c>
       <c r="BD14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BE14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BF14">
         <v>1</v>
@@ -3517,10 +3518,10 @@
         <v>1</v>
       </c>
       <c r="BH14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="BI14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BJ14">
         <v>2</v>
@@ -3529,10 +3530,10 @@
         <v>2</v>
       </c>
       <c r="BL14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="BM14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BN14">
         <v>1</v>
@@ -3541,9 +3542,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:67" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:67" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A15" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B15" s="9">
         <v>44642</v>
@@ -3552,31 +3553,31 @@
         <v>0.46875</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="M15" s="17">
+        <v>58</v>
+      </c>
+      <c r="M15" s="13">
         <v>0.37333333333333246</v>
       </c>
       <c r="N15" s="1">
@@ -3586,73 +3587,73 @@
         <v>12</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q15" s="1">
         <v>50</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U15" s="1">
         <v>8</v>
       </c>
       <c r="V15" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="X15" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z15" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AA15" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB15" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC15" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD15" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE15" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF15" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG15" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AH15" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AI15" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AJ15" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AK15" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AL15" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AM15">
         <v>20</v>
@@ -3670,10 +3671,10 @@
         <v>0</v>
       </c>
       <c r="AR15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AS15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AT15">
         <v>1</v>
@@ -3682,10 +3683,10 @@
         <v>1</v>
       </c>
       <c r="AV15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AW15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AX15">
         <v>1</v>
@@ -3694,10 +3695,10 @@
         <v>1</v>
       </c>
       <c r="AZ15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BA15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="BB15">
         <v>3</v>
@@ -3706,10 +3707,10 @@
         <v>1</v>
       </c>
       <c r="BD15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BE15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="BF15">
         <v>2</v>
@@ -3718,10 +3719,10 @@
         <v>1</v>
       </c>
       <c r="BH15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="BI15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BJ15">
         <v>1</v>
@@ -3730,10 +3731,10 @@
         <v>1</v>
       </c>
       <c r="BL15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="BM15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BN15">
         <v>1</v>
@@ -3742,9 +3743,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:67" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:67" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A16" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16" s="9">
         <v>44642</v>
@@ -3753,31 +3754,31 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J16" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K16" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="M16" s="17">
+        <v>58</v>
+      </c>
+      <c r="M16" s="13">
         <v>0.20000000000000048</v>
       </c>
       <c r="N16" s="1">
@@ -3787,73 +3788,73 @@
         <v>14</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="Q16" s="1">
         <v>50</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="T16" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U16" s="1">
         <v>50</v>
       </c>
       <c r="V16" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="W16" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="X16" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y16" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z16" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AA16" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB16" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC16" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD16" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE16" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF16" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG16" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AH16" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AI16" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AJ16" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AK16" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AL16" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AM16">
         <v>20</v>
@@ -3871,10 +3872,10 @@
         <v>0</v>
       </c>
       <c r="AR16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AS16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AT16">
         <v>1</v>
@@ -3883,10 +3884,10 @@
         <v>2</v>
       </c>
       <c r="AV16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AW16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AX16">
         <v>1</v>
@@ -3895,10 +3896,10 @@
         <v>1</v>
       </c>
       <c r="AZ16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BA16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="BB16">
         <v>1</v>
@@ -3907,10 +3908,10 @@
         <v>1</v>
       </c>
       <c r="BD16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BE16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="BF16">
         <v>1</v>
@@ -3919,10 +3920,10 @@
         <v>1</v>
       </c>
       <c r="BH16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BI16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="BJ16">
         <v>1</v>
@@ -3931,10 +3932,10 @@
         <v>1</v>
       </c>
       <c r="BL16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BM16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BN16">
         <v>2</v>
@@ -3943,9 +3944,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:67" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:67" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A17" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B17" s="9">
         <v>44642</v>
@@ -3954,31 +3955,31 @@
         <v>0.43402777777777773</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K17" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="M17" s="17">
+        <v>58</v>
+      </c>
+      <c r="M17" s="13">
         <v>1.6666666666666667</v>
       </c>
       <c r="N17" s="1">
@@ -3988,73 +3989,73 @@
         <v>8</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q17" s="1">
         <v>20</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U17" s="1">
         <v>50</v>
       </c>
       <c r="V17" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="W17" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="X17" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y17" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z17" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AA17" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB17" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC17" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD17" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE17" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF17" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG17" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AH17" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AI17" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AJ17" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AK17" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AL17" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AM17">
         <v>20</v>
@@ -4072,10 +4073,10 @@
         <v>0</v>
       </c>
       <c r="AR17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AS17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AT17">
         <v>1</v>
@@ -4084,10 +4085,10 @@
         <v>1</v>
       </c>
       <c r="AV17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AW17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AX17">
         <v>1</v>
@@ -4096,10 +4097,10 @@
         <v>1</v>
       </c>
       <c r="AZ17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BA17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="BB17">
         <v>1</v>
@@ -4108,10 +4109,10 @@
         <v>1</v>
       </c>
       <c r="BD17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BE17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="BF17">
         <v>1</v>
@@ -4120,10 +4121,10 @@
         <v>1</v>
       </c>
       <c r="BH17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BI17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="BJ17">
         <v>1</v>
@@ -4132,10 +4133,10 @@
         <v>2</v>
       </c>
       <c r="BL17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BM17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="BN17">
         <v>1</v>
@@ -4144,9 +4145,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:67" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:67" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A18" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B18" s="9">
         <v>44642</v>
@@ -4155,31 +4156,31 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J18" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K18" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="M18" s="17">
+        <v>58</v>
+      </c>
+      <c r="M18" s="13">
         <v>2.3333333333333326</v>
       </c>
       <c r="N18" s="1">
@@ -4189,73 +4190,73 @@
         <v>19</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q18" s="1">
         <v>50</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U18" s="1">
         <v>50</v>
       </c>
       <c r="V18" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="W18" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="X18" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y18" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z18" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AA18" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB18" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC18" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD18" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE18" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF18" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG18" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AH18" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AI18" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AJ18" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AK18" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AL18" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AM18">
         <v>20</v>
@@ -4273,10 +4274,10 @@
         <v>0</v>
       </c>
       <c r="AR18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AS18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AT18">
         <v>1</v>
@@ -4285,10 +4286,10 @@
         <v>2</v>
       </c>
       <c r="AV18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AW18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AX18">
         <v>1</v>
@@ -4297,10 +4298,10 @@
         <v>2</v>
       </c>
       <c r="AZ18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BA18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="BB18">
         <v>1</v>
@@ -4309,10 +4310,10 @@
         <v>2</v>
       </c>
       <c r="BD18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BE18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="BF18">
         <v>1</v>
@@ -4321,10 +4322,10 @@
         <v>2</v>
       </c>
       <c r="BH18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BI18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BJ18">
         <v>1</v>
@@ -4333,10 +4334,10 @@
         <v>1</v>
       </c>
       <c r="BL18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BM18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BN18">
         <v>1</v>
@@ -4345,9 +4346,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:67" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:67" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A19" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19" s="9">
         <v>44642</v>
@@ -4356,31 +4357,31 @@
         <v>0.61805555555555558</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J19" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="M19" s="17">
+        <v>58</v>
+      </c>
+      <c r="M19" s="13">
         <v>3</v>
       </c>
       <c r="N19" s="1">
@@ -4390,73 +4391,73 @@
         <v>15</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q19" s="1">
         <v>50</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="S19" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="T19" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U19" s="1">
         <v>30</v>
       </c>
       <c r="V19" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="W19" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="X19" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y19" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z19" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AA19" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB19" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC19" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD19" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE19" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF19" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG19" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AH19" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AI19" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AJ19" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AK19" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AL19" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AM19">
         <v>20</v>
@@ -4474,10 +4475,10 @@
         <v>0</v>
       </c>
       <c r="AR19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AS19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AT19">
         <v>1</v>
@@ -4486,10 +4487,10 @@
         <v>2</v>
       </c>
       <c r="AV19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AW19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AX19">
         <v>1</v>
@@ -4498,10 +4499,10 @@
         <v>2</v>
       </c>
       <c r="AZ19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BA19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="BB19">
         <v>1</v>
@@ -4510,10 +4511,10 @@
         <v>2</v>
       </c>
       <c r="BD19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BE19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="BF19">
         <v>1</v>
@@ -4522,10 +4523,10 @@
         <v>2</v>
       </c>
       <c r="BH19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BI19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BJ19">
         <v>1</v>
@@ -4534,10 +4535,10 @@
         <v>2</v>
       </c>
       <c r="BL19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BM19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BN19">
         <v>1</v>
@@ -4546,9 +4547,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:67" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:67" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A20" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" s="9">
         <v>44655</v>
@@ -4557,31 +4558,31 @@
         <v>0.5625</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J20" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K20" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="M20" s="17">
+        <v>58</v>
+      </c>
+      <c r="M20" s="13">
         <v>2.3333333333333335</v>
       </c>
       <c r="N20" s="1">
@@ -4591,73 +4592,73 @@
         <v>15</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q20" s="1">
         <v>50</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="T20" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U20" s="1">
         <v>3</v>
       </c>
       <c r="V20" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="W20" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="X20" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Y20" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z20" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AA20" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB20" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC20" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD20" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE20" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF20" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG20" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AH20" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AI20" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AJ20" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AK20" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AL20" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AM20">
         <v>20</v>
@@ -4675,10 +4676,10 @@
         <v>0</v>
       </c>
       <c r="AR20" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AS20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AT20">
         <v>1</v>
@@ -4687,10 +4688,10 @@
         <v>1</v>
       </c>
       <c r="AV20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AW20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AX20">
         <v>1</v>
@@ -4699,10 +4700,10 @@
         <v>1</v>
       </c>
       <c r="AZ20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BA20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BB20">
         <v>1</v>
@@ -4711,10 +4712,10 @@
         <v>2</v>
       </c>
       <c r="BD20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BE20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BF20">
         <v>1</v>
@@ -4723,10 +4724,10 @@
         <v>2</v>
       </c>
       <c r="BH20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BI20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BJ20">
         <v>2</v>
@@ -4735,10 +4736,10 @@
         <v>1</v>
       </c>
       <c r="BL20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BM20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BN20">
         <v>1</v>
@@ -4747,9 +4748,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:67" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:67" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A21" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B21" s="9">
         <v>44655</v>
@@ -4758,31 +4759,31 @@
         <v>0.53125</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J21" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K21" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="M21" s="17">
+        <v>58</v>
+      </c>
+      <c r="M21" s="13">
         <v>0.96000000000000074</v>
       </c>
       <c r="N21" s="1">
@@ -4792,73 +4793,73 @@
         <v>19</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q21" s="1">
         <v>50</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U21" s="1">
         <v>50</v>
       </c>
       <c r="V21" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="W21" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="X21" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y21" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z21" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AA21" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB21" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC21" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD21" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE21" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF21" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG21" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AH21" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AI21" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AJ21" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AK21" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AL21" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AM21">
         <v>20</v>
@@ -4876,10 +4877,10 @@
         <v>0</v>
       </c>
       <c r="AR21" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AS21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AT21">
         <v>2</v>
@@ -4888,10 +4889,10 @@
         <v>1</v>
       </c>
       <c r="AV21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AW21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AX21">
         <v>2</v>
@@ -4900,10 +4901,10 @@
         <v>1</v>
       </c>
       <c r="AZ21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BA21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="BB21">
         <v>2</v>
@@ -4912,10 +4913,10 @@
         <v>1</v>
       </c>
       <c r="BD21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BE21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="BF21">
         <v>2</v>
@@ -4924,10 +4925,10 @@
         <v>1</v>
       </c>
       <c r="BH21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BI21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BJ21">
         <v>1</v>
@@ -4936,10 +4937,10 @@
         <v>2</v>
       </c>
       <c r="BL21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BM21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BN21">
         <v>1</v>
@@ -4948,138 +4949,138 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:67" x14ac:dyDescent="0.6">
       <c r="F22" s="3"/>
       <c r="M22" s="3"/>
       <c r="P22" s="3"/>
       <c r="BO22" s="3"/>
     </row>
-    <row r="23" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:67" x14ac:dyDescent="0.6">
       <c r="F23" s="3"/>
       <c r="M23" s="3"/>
       <c r="P23" s="3"/>
       <c r="BO23" s="3"/>
     </row>
-    <row r="24" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:67" x14ac:dyDescent="0.6">
       <c r="F24" s="3"/>
       <c r="M24" s="3"/>
       <c r="P24" s="3"/>
       <c r="BO24" s="3"/>
     </row>
-    <row r="25" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:67" x14ac:dyDescent="0.6">
       <c r="F25" s="3"/>
       <c r="M25" s="3"/>
       <c r="P25" s="3"/>
       <c r="BO25" s="3"/>
     </row>
-    <row r="26" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:67" x14ac:dyDescent="0.6">
       <c r="F26" s="3"/>
       <c r="M26" s="3"/>
       <c r="P26" s="3"/>
       <c r="BO26" s="3"/>
     </row>
-    <row r="27" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:67" x14ac:dyDescent="0.6">
       <c r="F27" s="3"/>
       <c r="M27" s="3"/>
       <c r="P27" s="3"/>
       <c r="BO27" s="3"/>
     </row>
-    <row r="28" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:67" x14ac:dyDescent="0.6">
       <c r="F28" s="3"/>
       <c r="M28" s="3"/>
       <c r="P28" s="3"/>
       <c r="BO28" s="3"/>
     </row>
-    <row r="29" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:67" x14ac:dyDescent="0.6">
       <c r="F29" s="3"/>
       <c r="M29" s="3"/>
       <c r="P29" s="3"/>
       <c r="BO29" s="3"/>
     </row>
-    <row r="30" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:67" x14ac:dyDescent="0.6">
       <c r="F30" s="3"/>
       <c r="M30" s="3"/>
       <c r="P30" s="3"/>
       <c r="BO30" s="3"/>
     </row>
-    <row r="31" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:67" x14ac:dyDescent="0.6">
       <c r="F31" s="3"/>
       <c r="M31" s="3"/>
       <c r="P31" s="3"/>
       <c r="BO31" s="3"/>
     </row>
-    <row r="32" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:67" x14ac:dyDescent="0.6">
       <c r="F32" s="3"/>
       <c r="M32" s="3"/>
       <c r="BO32" s="3"/>
     </row>
-    <row r="33" spans="6:67" x14ac:dyDescent="0.25">
+    <row r="33" spans="6:67" x14ac:dyDescent="0.6">
       <c r="F33" s="3"/>
       <c r="BO33" s="3"/>
     </row>
-    <row r="34" spans="6:67" x14ac:dyDescent="0.25">
+    <row r="34" spans="6:67" x14ac:dyDescent="0.6">
       <c r="F34" s="3"/>
       <c r="BO34" s="3"/>
     </row>
-    <row r="35" spans="6:67" x14ac:dyDescent="0.25">
+    <row r="35" spans="6:67" x14ac:dyDescent="0.6">
       <c r="F35" s="3"/>
       <c r="BO35" s="3"/>
     </row>
-    <row r="36" spans="6:67" x14ac:dyDescent="0.25">
+    <row r="36" spans="6:67" x14ac:dyDescent="0.6">
       <c r="F36" s="3"/>
       <c r="BO36" s="3"/>
     </row>
-    <row r="37" spans="6:67" x14ac:dyDescent="0.25">
+    <row r="37" spans="6:67" x14ac:dyDescent="0.6">
       <c r="F37" s="3"/>
       <c r="BO37" s="3"/>
     </row>
-    <row r="38" spans="6:67" x14ac:dyDescent="0.25">
+    <row r="38" spans="6:67" x14ac:dyDescent="0.6">
       <c r="F38" s="3"/>
       <c r="BO38" s="3"/>
     </row>
-    <row r="39" spans="6:67" x14ac:dyDescent="0.25">
+    <row r="39" spans="6:67" x14ac:dyDescent="0.6">
       <c r="F39" s="3"/>
       <c r="BO39" s="3"/>
     </row>
-    <row r="40" spans="6:67" x14ac:dyDescent="0.25">
+    <row r="40" spans="6:67" x14ac:dyDescent="0.6">
       <c r="F40" s="3"/>
       <c r="BO40" s="3"/>
     </row>
-    <row r="41" spans="6:67" x14ac:dyDescent="0.25">
+    <row r="41" spans="6:67" x14ac:dyDescent="0.6">
       <c r="F41" s="3"/>
       <c r="BO41" s="3"/>
     </row>
-    <row r="42" spans="6:67" x14ac:dyDescent="0.25">
+    <row r="42" spans="6:67" x14ac:dyDescent="0.6">
       <c r="F42" s="3"/>
       <c r="BO42" s="3"/>
     </row>
-    <row r="43" spans="6:67" x14ac:dyDescent="0.25">
+    <row r="43" spans="6:67" x14ac:dyDescent="0.6">
       <c r="F43" s="3"/>
       <c r="BO43" s="3"/>
     </row>
-    <row r="44" spans="6:67" x14ac:dyDescent="0.25">
+    <row r="44" spans="6:67" x14ac:dyDescent="0.6">
       <c r="F44" s="3"/>
       <c r="BO44" s="3"/>
     </row>
-    <row r="45" spans="6:67" x14ac:dyDescent="0.25">
+    <row r="45" spans="6:67" x14ac:dyDescent="0.6">
       <c r="BO45" s="3"/>
     </row>
-    <row r="46" spans="6:67" x14ac:dyDescent="0.25">
+    <row r="46" spans="6:67" x14ac:dyDescent="0.6">
       <c r="BO46" s="3"/>
     </row>
-    <row r="47" spans="6:67" x14ac:dyDescent="0.25">
+    <row r="47" spans="6:67" x14ac:dyDescent="0.6">
       <c r="BO47" s="3"/>
     </row>
-    <row r="48" spans="6:67" x14ac:dyDescent="0.25">
+    <row r="48" spans="6:67" x14ac:dyDescent="0.6">
       <c r="BO48" s="3"/>
     </row>
-    <row r="49" spans="67:67" x14ac:dyDescent="0.25">
+    <row r="49" spans="67:67" x14ac:dyDescent="0.6">
       <c r="BO49" s="3"/>
     </row>
-    <row r="50" spans="67:67" x14ac:dyDescent="0.25">
+    <row r="50" spans="67:67" x14ac:dyDescent="0.6">
       <c r="BO50" s="3"/>
     </row>
-    <row r="51" spans="67:67" x14ac:dyDescent="0.25">
+    <row r="51" spans="67:67" x14ac:dyDescent="0.6">
       <c r="BO51" s="3"/>
     </row>
   </sheetData>

</xml_diff>